<commit_message>
token meer en excel bla
</commit_message>
<xml_diff>
--- a/Project5 Beoordeling.xlsx
+++ b/Project5 Beoordeling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7c2cf874958896d/Documenten/School Projecten/Leerjaar 2/Project5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{5BC9974A-03F9-4266-8911-E700F53468E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AB1540B-33F7-41BE-B04E-054A70B77253}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="13_ncr:1_{5BC9974A-03F9-4266-8911-E700F53468E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A158FAA3-0A7F-4253-9DCB-F020E13AD667}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="96">
   <si>
     <t>Groep1</t>
   </si>
@@ -917,10 +917,10 @@
   <dimension ref="A1:H97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="U82" sqref="U82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1022,8 +1022,12 @@
       <c r="E7" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="H7" s="7" t="s">
         <v>88</v>
       </c>
@@ -1035,8 +1039,12 @@
       <c r="E8" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="H8" s="7" t="s">
         <v>88</v>
       </c>
@@ -1045,18 +1053,24 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="43.2" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>88</v>
-      </c>
+      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -1074,9 +1088,7 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>88</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1466,7 +1478,7 @@
       </c>
       <c r="H38" s="8" t="str">
         <f t="shared" ref="H38" si="3">IF(COUNTIF(H39:H40,"v")+COUNTIF(H39:H40,"s")=2,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="39" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
@@ -1487,7 +1499,9 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="41" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
@@ -1903,7 +1917,7 @@
       </c>
       <c r="H79" s="1" t="str">
         <f>IF(COUNTIF(H80:H90,"v")+COUNTIF(H80:H90,"s")=8,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
     </row>
     <row r="80" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -1913,7 +1927,9 @@
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
+      <c r="H80" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="81" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B81" s="1" t="s">
@@ -1922,7 +1938,9 @@
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
-      <c r="H81" s="7"/>
+      <c r="H81" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="82" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B82" s="1" t="s">
@@ -1936,7 +1954,9 @@
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
-      <c r="H83" s="7"/>
+      <c r="H83" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="84" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="C84" s="2" t="s">
@@ -1945,7 +1965,9 @@
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
+      <c r="H84" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="85" spans="1:8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="C85" s="2" t="s">
@@ -1954,7 +1976,9 @@
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
+      <c r="H85" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="86" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B86" s="1" t="s">
@@ -1968,7 +1992,9 @@
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
+      <c r="H87" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="88" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B88" s="1" t="s">
@@ -1982,7 +2008,9 @@
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
-      <c r="H89" s="7"/>
+      <c r="H89" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="90" spans="1:8" ht="28.8" outlineLevel="2" x14ac:dyDescent="0.3">
       <c r="C90" s="2" t="s">
@@ -1991,7 +2019,9 @@
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
-      <c r="H90" s="7"/>
+      <c r="H90" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E91" s="1" t="s">

</xml_diff>